<commit_message>
Update NoTrace; update 24VDC cables
</commit_message>
<xml_diff>
--- a/Docs/AT-ETX-2i10G.CBL04_24V.xlsx
+++ b/Docs/AT-ETX-2i10G.CBL04_24V.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDocuments\ate\AutoTesters\TCL\ETX-2i-10G\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B45FD3-6766-41E9-8635-3C184C931728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38F0F8A-E11B-4A80-9CCA-BA703DA3BBAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5505" yWindow="1335" windowWidth="21600" windowHeight="13845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7335" yWindow="1725" windowWidth="20265" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -721,7 +721,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,7 +865,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="5">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="D25" s="18"/>
     </row>
@@ -932,12 +932,11 @@
         <v>15</v>
       </c>
       <c r="C32" s="3">
-        <f>C25</f>
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="D32" s="3">
         <f>$C$26*C32</f>
-        <v>800</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>